<commit_message>
Aula do dia 22/05
</commit_message>
<xml_diff>
--- a/EngenhariaDeSoftware/Trabalho1/Casos de teste para Importar no Word.xlsx
+++ b/EngenhariaDeSoftware/Trabalho1/Casos de teste para Importar no Word.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\engenhariadesoftware\EngenhariaDeSoftware\Trabalho1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="15">
   <si>
     <t>Entradas</t>
   </si>
@@ -50,18 +50,6 @@
     <t>Trabalhos</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>P2</t>
   </si>
   <si>
@@ -72,6 +60,15 @@
   </si>
   <si>
     <t>30/02/2019</t>
+  </si>
+  <si>
+    <t>Saida esperada</t>
+  </si>
+  <si>
+    <t>erro</t>
+  </si>
+  <si>
+    <t>positivo</t>
   </si>
 </sst>
 </file>
@@ -107,11 +104,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,23 +392,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D2" sqref="D2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -416,7 +424,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -433,25 +441,28 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>43511</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -459,25 +470,28 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>43511</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -485,25 +499,28 @@
       <c r="H4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>43511</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -511,25 +528,28 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>43511</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -537,22 +557,28 @@
       <c r="H6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" s="1">
         <v>43511</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>43510</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -560,22 +586,28 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" s="1">
         <v>43511</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>43510</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -583,22 +615,28 @@
       <c r="H8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" s="1">
         <v>43511</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
         <v>43510</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G9">
         <v>20</v>
@@ -606,22 +644,28 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10" s="1">
         <v>43511</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1">
         <v>43510</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <v>20</v>
@@ -629,137 +673,173 @@
       <c r="H10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11" s="1">
         <v>43511</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43516</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43511</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43516</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43511</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43516</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1">
-        <v>43516</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <v>43511</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43511</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43516</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43511</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1">
+        <v>43516</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="D12" s="1">
-        <v>43516</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <v>43511</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1">
-        <v>43516</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>20</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <v>43511</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43516</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14">
-        <v>20</v>
-      </c>
-      <c r="H14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <v>43511</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1">
-        <v>43516</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>43511</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1">
         <v>43516</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -767,22 +847,28 @@
       <c r="H16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17" s="1">
         <v>43511</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1">
         <v>43516</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G17">
         <v>20</v>
@@ -790,22 +876,28 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" s="1">
         <v>43511</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1">
         <v>43516</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G18">
         <v>20</v>
@@ -813,22 +905,28 @@
       <c r="H18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19" s="1">
         <v>43511</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1">
         <v>43516</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -836,22 +934,28 @@
       <c r="H19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" s="1">
         <v>43511</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1">
         <v>43516</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -859,22 +963,28 @@
       <c r="H20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" s="1">
         <v>43511</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1">
         <v>43516</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>20</v>
@@ -882,22 +992,28 @@
       <c r="H21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22" s="1">
         <v>43511</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1">
         <v>43516</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G22">
         <v>20</v>
@@ -905,22 +1021,28 @@
       <c r="H22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1">
         <v>43511</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
@@ -928,22 +1050,28 @@
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
         <v>43511</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -951,22 +1079,28 @@
       <c r="H24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1">
         <v>43511</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G25">
         <v>20</v>
@@ -974,22 +1108,28 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1">
         <v>43511</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G26">
         <v>20</v>
@@ -997,10 +1137,16 @@
       <c r="H26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1">
         <v>43511</v>
@@ -1009,10 +1155,10 @@
         <v>43510</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
@@ -1020,10 +1166,16 @@
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1">
         <v>43511</v>
@@ -1032,10 +1184,10 @@
         <v>43510</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1043,10 +1195,16 @@
       <c r="H28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1">
         <v>43511</v>
@@ -1055,10 +1213,10 @@
         <v>43510</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G29">
         <v>20</v>
@@ -1066,10 +1224,16 @@
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
       <c r="B30" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1">
         <v>43511</v>
@@ -1078,10 +1242,10 @@
         <v>43510</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>20</v>
@@ -1089,10 +1253,16 @@
       <c r="H30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
       <c r="B31" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1">
         <v>43511</v>
@@ -1101,10 +1271,10 @@
         <v>43516</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
@@ -1112,10 +1282,16 @@
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
       <c r="B32" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1">
         <v>43511</v>
@@ -1124,10 +1300,10 @@
         <v>43516</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1135,10 +1311,16 @@
       <c r="H32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>43511</v>
@@ -1147,10 +1329,10 @@
         <v>43516</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G33">
         <v>20</v>
@@ -1158,10 +1340,16 @@
       <c r="H33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
       <c r="B34" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1">
         <v>43511</v>
@@ -1170,10 +1358,10 @@
         <v>43516</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>20</v>
@@ -1181,22 +1369,28 @@
       <c r="H34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1">
         <v>43511</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E35" s="1">
         <v>43516</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G35" s="2">
         <v>0</v>
@@ -1204,22 +1398,28 @@
       <c r="H35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1">
         <v>43511</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E36" s="1">
         <v>43516</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1227,22 +1427,28 @@
       <c r="H36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
       <c r="B37" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1">
         <v>43511</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E37" s="1">
         <v>43516</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>20</v>
@@ -1250,22 +1456,28 @@
       <c r="H37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
       <c r="B38" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1">
         <v>43511</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
         <v>43516</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G38">
         <v>20</v>
@@ -1273,22 +1485,28 @@
       <c r="H38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
       <c r="B39" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1">
         <v>43511</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E39" s="1">
         <v>43516</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G39" s="2">
         <v>0</v>
@@ -1296,22 +1514,28 @@
       <c r="H39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
       <c r="B40" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1">
         <v>43511</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E40" s="1">
         <v>43516</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1319,22 +1543,28 @@
       <c r="H40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
       <c r="B41" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1">
         <v>43511</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E41" s="1">
         <v>43516</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G41">
         <v>20</v>
@@ -1342,22 +1572,28 @@
       <c r="H41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
       <c r="B42" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1">
         <v>43511</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E42" s="1">
         <v>43516</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G42">
         <v>20</v>
@@ -1365,8 +1601,14 @@
       <c r="H42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
       <c r="B43" s="1">
         <v>43511</v>
       </c>
@@ -1374,13 +1616,13 @@
         <v>43511</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G43" s="2">
         <v>0</v>
@@ -1388,8 +1630,14 @@
       <c r="H43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
       <c r="B44" s="1">
         <v>43511</v>
       </c>
@@ -1397,13 +1645,13 @@
         <v>43511</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -1411,8 +1659,14 @@
       <c r="H44">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
       <c r="B45" s="1">
         <v>43511</v>
       </c>
@@ -1420,13 +1674,13 @@
         <v>43511</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G45">
         <v>20</v>
@@ -1434,8 +1688,14 @@
       <c r="H45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
       <c r="B46" s="1">
         <v>43511</v>
       </c>
@@ -1443,13 +1703,13 @@
         <v>43511</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G46">
         <v>20</v>
@@ -1457,8 +1717,14 @@
       <c r="H46">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
       <c r="B47" s="1">
         <v>43511</v>
       </c>
@@ -1469,10 +1735,10 @@
         <v>43510</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G47" s="2">
         <v>0</v>
@@ -1480,8 +1746,14 @@
       <c r="H47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
       <c r="B48" s="1">
         <v>43511</v>
       </c>
@@ -1492,10 +1764,10 @@
         <v>43510</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1503,8 +1775,14 @@
       <c r="H48">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
       <c r="B49" s="1">
         <v>43511</v>
       </c>
@@ -1515,10 +1793,10 @@
         <v>43510</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G49">
         <v>20</v>
@@ -1526,8 +1804,14 @@
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
       <c r="B50" s="1">
         <v>43511</v>
       </c>
@@ -1538,10 +1822,10 @@
         <v>43510</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G50">
         <v>20</v>
@@ -1549,8 +1833,14 @@
       <c r="H50">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
       <c r="B51" s="1">
         <v>43511</v>
       </c>
@@ -1561,10 +1851,10 @@
         <v>43516</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G51" s="2">
         <v>0</v>
@@ -1572,8 +1862,14 @@
       <c r="H51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
       <c r="B52" s="1">
         <v>43511</v>
       </c>
@@ -1584,10 +1880,10 @@
         <v>43516</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -1595,8 +1891,14 @@
       <c r="H52">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
       <c r="B53" s="1">
         <v>43511</v>
       </c>
@@ -1607,10 +1909,10 @@
         <v>43516</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G53">
         <v>20</v>
@@ -1618,8 +1920,14 @@
       <c r="H53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
       <c r="B54" s="1">
         <v>43511</v>
       </c>
@@ -1630,10 +1938,10 @@
         <v>43516</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G54">
         <v>20</v>
@@ -1641,8 +1949,14 @@
       <c r="H54">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
       <c r="B55" s="1">
         <v>43511</v>
       </c>
@@ -1650,13 +1964,13 @@
         <v>43511</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E55" s="1">
         <v>43516</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G55" s="2">
         <v>0</v>
@@ -1664,8 +1978,14 @@
       <c r="H55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
       <c r="B56" s="1">
         <v>43511</v>
       </c>
@@ -1673,13 +1993,13 @@
         <v>43511</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1">
         <v>43516</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1687,8 +2007,14 @@
       <c r="H56">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
       <c r="B57" s="1">
         <v>43511</v>
       </c>
@@ -1696,13 +2022,13 @@
         <v>43511</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1">
         <v>43516</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G57">
         <v>20</v>
@@ -1710,8 +2036,14 @@
       <c r="H57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
       <c r="B58" s="1">
         <v>43511</v>
       </c>
@@ -1719,13 +2051,13 @@
         <v>43511</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1">
         <v>43516</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G58">
         <v>20</v>
@@ -1733,8 +2065,14 @@
       <c r="H58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
       <c r="B59" s="1">
         <v>43511</v>
       </c>
@@ -1742,13 +2080,13 @@
         <v>43511</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E59" s="1">
         <v>43516</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G59" s="2">
         <v>0</v>
@@ -1756,8 +2094,14 @@
       <c r="H59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
       <c r="B60" s="1">
         <v>43511</v>
       </c>
@@ -1765,13 +2109,13 @@
         <v>43511</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E60" s="1">
         <v>43516</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -1779,8 +2123,14 @@
       <c r="H60">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
       <c r="B61" s="1">
         <v>43511</v>
       </c>
@@ -1788,13 +2138,13 @@
         <v>43511</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E61" s="1">
         <v>43516</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G61">
         <v>20</v>
@@ -1802,8 +2152,14 @@
       <c r="H61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
       <c r="B62" s="1">
         <v>43511</v>
       </c>
@@ -1811,13 +2167,13 @@
         <v>43511</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E62" s="1">
         <v>43516</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G62">
         <v>20</v>
@@ -1825,22 +2181,28 @@
       <c r="H62">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G63" s="2">
         <v>0</v>
@@ -1848,22 +2210,28 @@
       <c r="H63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -1871,22 +2239,28 @@
       <c r="H64">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G65">
         <v>20</v>
@@ -1894,22 +2268,28 @@
       <c r="H65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G66">
         <v>20</v>
@@ -1917,22 +2297,28 @@
       <c r="H66">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D67" s="1">
         <v>43510</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G67" s="2">
         <v>0</v>
@@ -1940,22 +2326,28 @@
       <c r="H67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D68" s="1">
         <v>43510</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -1963,22 +2355,28 @@
       <c r="H68">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D69" s="1">
         <v>43510</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G69">
         <v>20</v>
@@ -1986,22 +2384,28 @@
       <c r="H69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
       <c r="B70" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D70" s="1">
         <v>43510</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G70">
         <v>20</v>
@@ -2009,22 +2413,28 @@
       <c r="H70">
         <v>8</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D71" s="1">
         <v>43516</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G71" s="2">
         <v>0</v>
@@ -2032,22 +2442,28 @@
       <c r="H71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D72" s="1">
         <v>43516</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -2055,22 +2471,28 @@
       <c r="H72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D73" s="1">
         <v>43516</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G73">
         <v>20</v>
@@ -2078,22 +2500,28 @@
       <c r="H73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D74" s="1">
         <v>43516</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G74">
         <v>20</v>
@@ -2101,22 +2529,28 @@
       <c r="H74">
         <v>8</v>
       </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E75" s="1">
         <v>43516</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G75" s="2">
         <v>0</v>
@@ -2124,22 +2558,28 @@
       <c r="H75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E76" s="1">
         <v>43516</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -2147,22 +2587,28 @@
       <c r="H76">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E77" s="1">
         <v>43516</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G77">
         <v>20</v>
@@ -2170,22 +2616,28 @@
       <c r="H77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E78" s="1">
         <v>43516</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G78">
         <v>20</v>
@@ -2193,22 +2645,28 @@
       <c r="H78">
         <v>8</v>
       </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E79" s="1">
         <v>43516</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G79" s="2">
         <v>0</v>
@@ -2216,22 +2674,28 @@
       <c r="H79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E80" s="1">
         <v>43516</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -2239,22 +2703,28 @@
       <c r="H80">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E81" s="1">
         <v>43516</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G81">
         <v>20</v>
@@ -2262,28 +2732,37 @@
       <c r="H81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E82" s="1">
         <v>43516</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G82">
         <v>20</v>
       </c>
       <c r="H82">
         <v>8</v>
+      </c>
+      <c r="J82" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="1048576" spans="2:4" x14ac:dyDescent="0.25">
@@ -2291,6 +2770,9 @@
       <c r="D1048576" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>